<commit_message>
Revisited enemy prefab setup, AI, and navigation system
Still highly considering revamping navigation system. Current implementation is stable with occasional pathing bug (seems to use old path instead of updated one)
</commit_message>
<xml_diff>
--- a/Design Docs/Spells.xlsx
+++ b/Design Docs/Spells.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1046ECE2-3B8F-4719-8018-36BEAD95A3FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70956A4-32E8-4B55-9073-108EBE3C5B3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casting Method" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Explosion</t>
   </si>
   <si>
-    <t>Explodes. Yep.</t>
-  </si>
-  <si>
     <t>Mesh changer</t>
   </si>
   <si>
@@ -163,6 +160,15 @@
   </si>
   <si>
     <t>Reduces the amount of mana a spell consumes</t>
+  </si>
+  <si>
+    <t>Bouncing Projectile</t>
+  </si>
+  <si>
+    <t>Ricochets off walls</t>
+  </si>
+  <si>
+    <t>Explodes. Yep. Applies other effects in spell.</t>
   </si>
 </sst>
 </file>
@@ -644,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93ED70A4-E6B4-4236-9250-11F042C2E2B5}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,7 +748,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -752,10 +758,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446AC232-E605-413C-B98C-0ABD243CEB14}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,10 +784,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
@@ -789,26 +795,34 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>46</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bullrush and bug fixes
</commit_message>
<xml_diff>
--- a/Design Docs/Spells.xlsx
+++ b/Design Docs/Spells.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70956A4-32E8-4B55-9073-108EBE3C5B3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB921720-A8EE-48EA-9955-3AA2E6912B90}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casting Method" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -169,6 +169,27 @@
   </si>
   <si>
     <t>Explodes. Yep. Applies other effects in spell.</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Puts target to sleep state. Taking damage will aggro</t>
+  </si>
+  <si>
+    <t>Bullrush</t>
+  </si>
+  <si>
+    <t>Target will burst forward certain distance depending on power</t>
+  </si>
+  <si>
+    <t>Boost Attack Power</t>
+  </si>
+  <si>
+    <t>Boost Defense</t>
+  </si>
+  <si>
+    <t>Spawn Minion</t>
   </si>
 </sst>
 </file>
@@ -558,7 +579,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,16 +669,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93ED70A4-E6B4-4236-9250-11F042C2E2B5}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="2" max="2" width="57.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -749,6 +770,37 @@
       </c>
       <c r="B11" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved loot system and UI updates
Removed some debug logs
Added 1st pass official loot config assets
</commit_message>
<xml_diff>
--- a/Design Docs/Spells.xlsx
+++ b/Design Docs/Spells.xlsx
@@ -3,14 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB921720-A8EE-48EA-9955-3AA2E6912B90}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8362F1-5E3C-425D-9D55-B5ABBA04E8C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Casting Method" sheetId="1" r:id="rId1"/>
-    <sheet name="OnHit Effect" sheetId="2" r:id="rId2"/>
-    <sheet name="Spell Modifiers" sheetId="3" r:id="rId3"/>
+    <sheet name="Player Stats" sheetId="5" r:id="rId1"/>
+    <sheet name="Casting Method" sheetId="1" r:id="rId2"/>
+    <sheet name="Spell Effects" sheetId="7" r:id="rId3"/>
+    <sheet name="Spell Modifiers" sheetId="3" r:id="rId4"/>
+    <sheet name="Casting Method Ideas" sheetId="6" r:id="rId5"/>
+    <sheet name="Spell Effect Ideas" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -33,51 +36,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Straight Shot</t>
-  </si>
-  <si>
-    <t>Lob Shot</t>
-  </si>
-  <si>
-    <t>Spread Shot</t>
-  </si>
-  <si>
-    <t>Radial Spread Shot</t>
-  </si>
-  <si>
-    <t>Short Radius Explosion</t>
-  </si>
-  <si>
-    <t>Applies effect upon self</t>
-  </si>
-  <si>
-    <t>Fires a single projectile directly forward</t>
-  </si>
-  <si>
-    <t>Fires a single projectile that is affected by gravity</t>
-  </si>
-  <si>
-    <t>Fires multiple projectiles in a general direction</t>
-  </si>
-  <si>
-    <t>Beam</t>
-  </si>
-  <si>
-    <t>Fires multiple projectiles in random directions around the user</t>
-  </si>
-  <si>
-    <t>Area of effect</t>
-  </si>
-  <si>
-    <t>Constant ray</t>
-  </si>
-  <si>
-    <t>Magic Missile</t>
-  </si>
-  <si>
-    <t>Deals damage</t>
-  </si>
-  <si>
     <t>Heal</t>
   </si>
   <si>
@@ -99,12 +57,6 @@
     <t>Spell Spawn</t>
   </si>
   <si>
-    <t>Shield</t>
-  </si>
-  <si>
-    <t>Maintained area around user that triggers when damageable object enters radius</t>
-  </si>
-  <si>
     <t>Poison</t>
   </si>
   <si>
@@ -190,6 +142,336 @@
   </si>
   <si>
     <t>Spawn Minion</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Self Instant I</t>
+  </si>
+  <si>
+    <t>Interval(seconds)</t>
+  </si>
+  <si>
+    <t>Self Instant II</t>
+  </si>
+  <si>
+    <t>Self Instant III</t>
+  </si>
+  <si>
+    <t>Self Instant IV</t>
+  </si>
+  <si>
+    <t>CM_Self_Instant_1</t>
+  </si>
+  <si>
+    <t>CM_Self_Instant_2</t>
+  </si>
+  <si>
+    <t>CM_Self_Instant_3</t>
+  </si>
+  <si>
+    <t>CM_Self_Instant_4</t>
+  </si>
+  <si>
+    <t>Player Max HP</t>
+  </si>
+  <si>
+    <t>Player Max MP</t>
+  </si>
+  <si>
+    <t>Player Speed</t>
+  </si>
+  <si>
+    <t>MP Recharge Rate</t>
+  </si>
+  <si>
+    <t>1s / Recharge</t>
+  </si>
+  <si>
+    <t>Self Held I</t>
+  </si>
+  <si>
+    <t>Self Held II</t>
+  </si>
+  <si>
+    <t>Self Held III</t>
+  </si>
+  <si>
+    <t>Self Held IV</t>
+  </si>
+  <si>
+    <t>CM_Self_Held_1</t>
+  </si>
+  <si>
+    <t>CM_Self_Held_2</t>
+  </si>
+  <si>
+    <t>CM_Self_Held_3</t>
+  </si>
+  <si>
+    <t>CM_Self_Held_4</t>
+  </si>
+  <si>
+    <t>Casts spell upon self per click</t>
+  </si>
+  <si>
+    <t>Casts spell upon self while shoot input is held</t>
+  </si>
+  <si>
+    <t>Power Mod</t>
+  </si>
+  <si>
+    <t>Self Charge I</t>
+  </si>
+  <si>
+    <t>CM_Self_Charge_1</t>
+  </si>
+  <si>
+    <t>Self Charge II</t>
+  </si>
+  <si>
+    <t>Self Charge III</t>
+  </si>
+  <si>
+    <t>Self Charge IV</t>
+  </si>
+  <si>
+    <t>CM_Self_Charge_2</t>
+  </si>
+  <si>
+    <t>CM_Self_Charge_3</t>
+  </si>
+  <si>
+    <t>CM_Self_Charge_4</t>
+  </si>
+  <si>
+    <t>Casts spell upon self when shoot input is released</t>
+  </si>
+  <si>
+    <t>Single Shot Instant I</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Instant_1</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Instant_2</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Instant_3</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Instant_4</t>
+  </si>
+  <si>
+    <t>Single Shot Instant II</t>
+  </si>
+  <si>
+    <t>Single Shot Instant III</t>
+  </si>
+  <si>
+    <t>Single Shot Instant IV</t>
+  </si>
+  <si>
+    <t>Fires a projectile that will deliver effects per click</t>
+  </si>
+  <si>
+    <t>Single Shot Held I</t>
+  </si>
+  <si>
+    <t>Single Shot Held II</t>
+  </si>
+  <si>
+    <t>Single Shot Held III</t>
+  </si>
+  <si>
+    <t>Single Shot Held IV</t>
+  </si>
+  <si>
+    <t>Fires projectiles that will deliver effects while shoot input is held</t>
+  </si>
+  <si>
+    <t>Single shot</t>
+  </si>
+  <si>
+    <t>Spread shot</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Lobbed shot</t>
+  </si>
+  <si>
+    <t>Single Shot Charge I</t>
+  </si>
+  <si>
+    <t>Single Shot Charge II</t>
+  </si>
+  <si>
+    <t>Single Shot Charge III</t>
+  </si>
+  <si>
+    <t>Single Shot Charge IV</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Held_1</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Held_2</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Held_3</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Held_4</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Charge_1</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Charge_2</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Charge_3</t>
+  </si>
+  <si>
+    <t>CM_SingleShot_Charge_4</t>
+  </si>
+  <si>
+    <t>Fires a projectile that will deliver effects when shoot input is released</t>
+  </si>
+  <si>
+    <t>Spread Shot Instant I</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Instant_1</t>
+  </si>
+  <si>
+    <t>Spread Shot Instant II</t>
+  </si>
+  <si>
+    <t>Spread Shot Instant III</t>
+  </si>
+  <si>
+    <t>Spread Shot Instant IV</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Instant_2</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Instant_3</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Instant_4</t>
+  </si>
+  <si>
+    <t>Fires several projectiles that will deliver effects per click</t>
+  </si>
+  <si>
+    <t>Special?</t>
+  </si>
+  <si>
+    <t>Spread Shot Held I</t>
+  </si>
+  <si>
+    <t>Spread Shot Held II</t>
+  </si>
+  <si>
+    <t>Spread Shot Held III</t>
+  </si>
+  <si>
+    <t>Spread Shot Held IV</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Held_1</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Held_2</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Held_3</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Held_4</t>
+  </si>
+  <si>
+    <t>Fires several projectiles that will deliver effects while shoot input is held</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Damage I</t>
+  </si>
+  <si>
+    <t>Effect_Damage_1</t>
+  </si>
+  <si>
+    <t>Effect_Damage_2</t>
+  </si>
+  <si>
+    <t>Effect_Damage_3</t>
+  </si>
+  <si>
+    <t>Effect_Damage_4</t>
+  </si>
+  <si>
+    <t>Damage II</t>
+  </si>
+  <si>
+    <t>Damage III</t>
+  </si>
+  <si>
+    <t>Damage IV</t>
+  </si>
+  <si>
+    <t>Deals normal damage to enemy</t>
+  </si>
+  <si>
+    <t>Boost Speed</t>
+  </si>
+  <si>
+    <t>Drain</t>
+  </si>
+  <si>
+    <t>Health is restored to caster</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Deals damage (can be elemental)</t>
+  </si>
+  <si>
+    <t>Spread Shot Charge I</t>
+  </si>
+  <si>
+    <t>Spread Shot Charge II</t>
+  </si>
+  <si>
+    <t>Spread Shot Charge III</t>
+  </si>
+  <si>
+    <t>Spread Shot Charge IV</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Charge_1</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Charge_2</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Charge_3</t>
+  </si>
+  <si>
+    <t>CM_SpreadShot_Charge_4</t>
+  </si>
+  <si>
+    <t>Fires several projectiles that will deliver effects when shoot input is released</t>
   </si>
 </sst>
 </file>
@@ -575,90 +857,775 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74536ACF-E41D-40A5-B8D5-7E90D20B5098}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="68.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="24.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G26" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G27" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G28" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G29" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G30" s="3">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G31" s="3">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="3">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G33" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="G35" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G36" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="G37" s="3">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -667,140 +1634,78 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93ED70A4-E6B4-4236-9250-11F042C2E2B5}">
-  <dimension ref="A1:C16"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57D3610-B5A4-41AC-BDAB-66106124F19C}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="2" width="57.44140625" customWidth="1"/>
+    <col min="1" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="56.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -808,7 +1713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446AC232-E605-413C-B98C-0ABD243CEB14}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -831,15 +1736,15 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
@@ -847,38 +1752,247 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C79084-3309-4E88-976D-CB785F398913}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93ED70A4-E6B4-4236-9250-11F042C2E2B5}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="57.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing UI and physics bugs
</commit_message>
<xml_diff>
--- a/Design Docs/Spells.xlsx
+++ b/Design Docs/Spells.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552446BE-9071-4B30-8190-DB1B2566BA76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A4E955-0D69-4BA3-86A3-B4AAC44D13BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player Stats" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="158">
   <si>
     <t>Name</t>
   </si>
@@ -472,13 +472,40 @@
   </si>
   <si>
     <t>Fires several projectiles that will deliver effects when shoot input is released</t>
+  </si>
+  <si>
+    <t>Summon Skeleton I</t>
+  </si>
+  <si>
+    <t>Summon Skeleton II</t>
+  </si>
+  <si>
+    <t>Summon Skeleton III</t>
+  </si>
+  <si>
+    <t>Summon Skeleton IV</t>
+  </si>
+  <si>
+    <t>Effect_Summon_Skeleton_1</t>
+  </si>
+  <si>
+    <t>Effect_Summon_Skeleton_2</t>
+  </si>
+  <si>
+    <t>Effect_Summon_Skeleton_3</t>
+  </si>
+  <si>
+    <t>Effect_Summon_Skeleton_4</t>
+  </si>
+  <si>
+    <t>Summons a skeleton warrior</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,6 +518,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -864,13 +897,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -878,7 +911,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -886,7 +919,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -894,7 +927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -914,21 +947,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="68.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="24.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -951,7 +984,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -968,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -985,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -1002,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
@@ -1020,7 +1053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>54</v>
       </c>
@@ -1038,7 +1071,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>55</v>
       </c>
@@ -1056,7 +1089,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
@@ -1074,7 +1107,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
@@ -1092,7 +1125,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>65</v>
       </c>
@@ -1110,7 +1143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
@@ -1128,7 +1161,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>68</v>
       </c>
@@ -1146,7 +1179,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>69</v>
       </c>
@@ -1164,7 +1197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>74</v>
       </c>
@@ -1182,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>79</v>
       </c>
@@ -1200,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>80</v>
       </c>
@@ -1218,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>81</v>
       </c>
@@ -1236,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>83</v>
       </c>
@@ -1254,7 +1287,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>84</v>
       </c>
@@ -1272,7 +1305,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>85</v>
       </c>
@@ -1290,7 +1323,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>86</v>
       </c>
@@ -1308,7 +1341,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>93</v>
       </c>
@@ -1326,7 +1359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>94</v>
       </c>
@@ -1344,7 +1377,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>95</v>
       </c>
@@ -1362,7 +1395,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>96</v>
       </c>
@@ -1380,7 +1413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>106</v>
       </c>
@@ -1401,7 +1434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>108</v>
       </c>
@@ -1422,7 +1455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>109</v>
       </c>
@@ -1443,7 +1476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>110</v>
       </c>
@@ -1464,7 +1497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>116</v>
       </c>
@@ -1485,7 +1518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>117</v>
       </c>
@@ -1506,7 +1539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>118</v>
       </c>
@@ -1527,7 +1560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>119</v>
       </c>
@@ -1548,7 +1581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>140</v>
       </c>
@@ -1568,7 +1601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>141</v>
       </c>
@@ -1588,7 +1621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>142</v>
       </c>
@@ -1608,7 +1641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>143</v>
       </c>
@@ -1636,21 +1669,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57D3610-B5A4-41AC-BDAB-66106124F19C}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="56.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1667,7 +1701,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -1684,31 +1718,127 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
       <c r="B4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
       <c r="B5" t="s">
         <v>130</v>
       </c>
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9">
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1721,14 +1851,14 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="54.88671875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -1750,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -1758,7 +1888,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1766,7 +1896,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1774,7 +1904,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
@@ -1796,42 +1926,42 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -1847,17 +1977,17 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="2" width="57.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1868,7 +1998,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -1876,7 +2006,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1884,7 +2014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1892,7 +2022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1900,7 +2030,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1908,7 +2038,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1916,7 +2046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1924,7 +2054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1932,7 +2062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1940,7 +2070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1948,7 +2078,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1956,7 +2086,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1964,27 +2094,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>136</v>
       </c>

</xml_diff>